<commit_message>
Überarbeitung der Auswertung der Wasserstände
</commit_message>
<xml_diff>
--- a/Wasser/Tabelle Wassertiefe.xlsx
+++ b/Wasser/Tabelle Wassertiefe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandra\Documents\GitHub\Moore-Lichtenau-Meusebach\Wasser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28C1C22-E4F3-4B55-8562-9789C7E16219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC66CDC-7F27-432A-B4DC-BDAA4650F825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DF3E7877-1137-4C85-8A00-0D067A96282D}"/>
   </bookViews>
@@ -101,11 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -448,32 +447,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22E4409-4333-4157-8A52-B4816E7E77F5}">
   <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="4" max="4" width="11.42578125" style="4"/>
-    <col min="5" max="5" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="11.42578125" style="3"/>
+    <col min="4" max="4" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -481,17 +479,17 @@
       <c r="A2" s="1">
         <v>45799</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="str">
+      <c r="D2" s="3" t="str">
         <f>B2&amp;C2</f>
         <v>MT1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>19</v>
       </c>
     </row>
@@ -499,17 +497,17 @@
       <c r="A3" s="1">
         <v>45799</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="str">
+      <c r="D3" s="3" t="str">
         <f t="shared" ref="D3:D66" si="0">B3&amp;C3</f>
         <v>MT2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>6.5</v>
       </c>
     </row>
@@ -517,17 +515,17 @@
       <c r="A4" s="1">
         <v>45799</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="str">
+      <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>20.5</v>
       </c>
     </row>
@@ -535,17 +533,17 @@
       <c r="A5" s="1">
         <v>45799</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="str">
+      <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>10</v>
       </c>
     </row>
@@ -553,17 +551,17 @@
       <c r="A6" s="1">
         <v>45799</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" s="4" t="str">
+      <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>9</v>
       </c>
     </row>
@@ -571,17 +569,17 @@
       <c r="A7" s="1">
         <v>45799</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="str">
+      <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>18</v>
       </c>
     </row>
@@ -589,17 +587,17 @@
       <c r="A8" s="1">
         <v>45799</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="4" t="str">
+      <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>19</v>
       </c>
     </row>
@@ -607,17 +605,17 @@
       <c r="A9" s="1">
         <v>45799</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="str">
+      <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L3</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>10</v>
       </c>
     </row>
@@ -625,17 +623,17 @@
       <c r="A10" s="1">
         <v>45799</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="str">
+      <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L4</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>0</v>
       </c>
     </row>
@@ -643,17 +641,17 @@
       <c r="A11" s="1">
         <v>45811</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="4" t="str">
+      <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>24</v>
       </c>
     </row>
@@ -661,17 +659,17 @@
       <c r="A12" s="1">
         <v>45811</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="4" t="str">
+      <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT2</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>18</v>
       </c>
     </row>
@@ -679,17 +677,17 @@
       <c r="A13" s="1">
         <v>45811</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="4" t="str">
+      <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN1</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>30</v>
       </c>
     </row>
@@ -697,17 +695,17 @@
       <c r="A14" s="1">
         <v>45811</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="4" t="str">
+      <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN2</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
         <v>18</v>
       </c>
     </row>
@@ -715,17 +713,17 @@
       <c r="A15" s="1">
         <v>45811</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="4" t="str">
+      <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN3</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>20</v>
       </c>
     </row>
@@ -733,17 +731,17 @@
       <c r="A16" s="1">
         <v>45811</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="4" t="str">
+      <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L1</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>23</v>
       </c>
     </row>
@@ -751,17 +749,17 @@
       <c r="A17" s="1">
         <v>45811</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="4" t="str">
+      <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L2</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
         <v>21</v>
       </c>
     </row>
@@ -769,17 +767,17 @@
       <c r="A18" s="1">
         <v>45811</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" s="4" t="str">
+      <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L3</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>16</v>
       </c>
     </row>
@@ -787,17 +785,17 @@
       <c r="A19" s="1">
         <v>45811</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="D19" s="4" t="str">
+      <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L4</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19">
         <v>4.5</v>
       </c>
     </row>
@@ -805,17 +803,17 @@
       <c r="A20" s="1">
         <v>45821</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="4" t="str">
+      <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT1</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20">
         <v>16</v>
       </c>
     </row>
@@ -823,17 +821,17 @@
       <c r="A21" s="1">
         <v>45821</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="4" t="str">
+      <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT2</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21">
         <v>8</v>
       </c>
     </row>
@@ -841,17 +839,17 @@
       <c r="A22" s="1">
         <v>45821</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="4" t="str">
+      <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN1</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22">
         <v>24</v>
       </c>
     </row>
@@ -859,17 +857,17 @@
       <c r="A23" s="1">
         <v>45821</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="4" t="str">
+      <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN2</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23">
         <v>12</v>
       </c>
     </row>
@@ -877,17 +875,17 @@
       <c r="A24" s="1">
         <v>45821</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" s="4" t="str">
+      <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN3</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24">
         <v>16</v>
       </c>
     </row>
@@ -895,17 +893,17 @@
       <c r="A25" s="1">
         <v>45821</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="4" t="str">
+      <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L1</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25">
         <v>20</v>
       </c>
     </row>
@@ -913,17 +911,17 @@
       <c r="A26" s="1">
         <v>45821</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
-      <c r="D26" s="4" t="str">
+      <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L2</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>17</v>
       </c>
     </row>
@@ -931,17 +929,17 @@
       <c r="A27" s="1">
         <v>45821</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
-      <c r="D27" s="4" t="str">
+      <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L3</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27">
         <v>10</v>
       </c>
     </row>
@@ -949,17 +947,17 @@
       <c r="A28" s="1">
         <v>45821</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
-      <c r="D28" s="4" t="str">
+      <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L4</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28">
         <v>0</v>
       </c>
     </row>
@@ -967,17 +965,17 @@
       <c r="A29" s="1">
         <v>45824</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="4" t="str">
+      <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT1</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29">
         <v>40</v>
       </c>
     </row>
@@ -985,17 +983,17 @@
       <c r="A30" s="1">
         <v>45824</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
-      <c r="D30" s="4" t="str">
+      <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT2</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30">
         <v>35</v>
       </c>
     </row>
@@ -1003,17 +1001,17 @@
       <c r="A31" s="1">
         <v>45824</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="4" t="str">
+      <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN1</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31">
         <v>40</v>
       </c>
     </row>
@@ -1021,17 +1019,17 @@
       <c r="A32" s="1">
         <v>45824</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
-      <c r="D32" s="4" t="str">
+      <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN2</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32">
         <v>20.5</v>
       </c>
     </row>
@@ -1039,17 +1037,17 @@
       <c r="A33" s="1">
         <v>45824</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C33">
         <v>3</v>
       </c>
-      <c r="D33" s="4" t="str">
+      <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN3</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33">
         <v>25</v>
       </c>
     </row>
@@ -1057,17 +1055,17 @@
       <c r="A34" s="1">
         <v>45824</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" s="4" t="str">
+      <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L1</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34">
         <v>29</v>
       </c>
     </row>
@@ -1075,17 +1073,17 @@
       <c r="A35" s="1">
         <v>45824</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
-      <c r="D35" s="4" t="str">
+      <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L2</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35">
         <v>24</v>
       </c>
     </row>
@@ -1093,17 +1091,17 @@
       <c r="A36" s="1">
         <v>45824</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
-      <c r="D36" s="4" t="str">
+      <c r="D36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L3</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36">
         <v>26.5</v>
       </c>
     </row>
@@ -1111,17 +1109,17 @@
       <c r="A37" s="1">
         <v>45824</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
-      <c r="D37" s="4" t="str">
+      <c r="D37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L4</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37">
         <v>9</v>
       </c>
     </row>
@@ -1129,17 +1127,17 @@
       <c r="A38" s="1">
         <v>45832</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" s="4" t="str">
+      <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT1</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38">
         <v>27</v>
       </c>
     </row>
@@ -1147,17 +1145,17 @@
       <c r="A39" s="1">
         <v>45832</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
-      <c r="D39" s="4" t="str">
+      <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT2</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39">
         <v>20</v>
       </c>
     </row>
@@ -1165,17 +1163,17 @@
       <c r="A40" s="1">
         <v>45832</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
-      <c r="D40" s="4" t="str">
+      <c r="D40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN1</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40">
         <v>34</v>
       </c>
     </row>
@@ -1183,17 +1181,17 @@
       <c r="A41" s="1">
         <v>45832</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
-      <c r="D41" s="4" t="str">
+      <c r="D41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN2</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41">
         <v>20</v>
       </c>
     </row>
@@ -1201,17 +1199,17 @@
       <c r="A42" s="1">
         <v>45832</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C42">
         <v>3</v>
       </c>
-      <c r="D42" s="4" t="str">
+      <c r="D42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN3</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42">
         <v>24</v>
       </c>
     </row>
@@ -1219,17 +1217,17 @@
       <c r="A43" s="1">
         <v>45832</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="D43" s="4" t="str">
+      <c r="D43" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L1</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43">
         <v>19</v>
       </c>
     </row>
@@ -1237,17 +1235,17 @@
       <c r="A44" s="1">
         <v>45832</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
-      <c r="D44" s="4" t="str">
+      <c r="D44" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L2</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44">
         <v>14</v>
       </c>
     </row>
@@ -1255,17 +1253,17 @@
       <c r="A45" s="1">
         <v>45832</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C45">
         <v>3</v>
       </c>
-      <c r="D45" s="4" t="str">
+      <c r="D45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L3</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45">
         <v>9</v>
       </c>
     </row>
@@ -1273,17 +1271,17 @@
       <c r="A46" s="1">
         <v>45832</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
-      <c r="D46" s="4" t="str">
+      <c r="D46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L4</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46">
         <v>0</v>
       </c>
     </row>
@@ -1291,17 +1289,17 @@
       <c r="A47" s="1">
         <v>45842</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="D47" s="4" t="str">
+      <c r="D47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT1</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47">
         <v>18</v>
       </c>
     </row>
@@ -1309,17 +1307,17 @@
       <c r="A48" s="1">
         <v>45842</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
-      <c r="D48" s="4" t="str">
+      <c r="D48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT2</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48">
         <v>1</v>
       </c>
     </row>
@@ -1327,17 +1325,17 @@
       <c r="A49" s="1">
         <v>45842</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="D49" s="4" t="str">
+      <c r="D49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN1</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49">
         <v>22</v>
       </c>
     </row>
@@ -1345,17 +1343,17 @@
       <c r="A50" s="1">
         <v>45842</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
-      <c r="D50" s="4" t="str">
+      <c r="D50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN2</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50">
         <v>9</v>
       </c>
     </row>
@@ -1363,17 +1361,17 @@
       <c r="A51" s="1">
         <v>45842</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
-      <c r="D51" s="4" t="str">
+      <c r="D51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN3</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51">
         <v>12</v>
       </c>
     </row>
@@ -1381,17 +1379,17 @@
       <c r="A52" s="1">
         <v>45842</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
-      <c r="D52" s="4" t="str">
+      <c r="D52" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L1</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52">
         <v>4</v>
       </c>
     </row>
@@ -1399,17 +1397,17 @@
       <c r="A53" s="1">
         <v>45842</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
-      <c r="D53" s="4" t="str">
+      <c r="D53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L2</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53">
         <v>3</v>
       </c>
     </row>
@@ -1417,17 +1415,17 @@
       <c r="A54" s="1">
         <v>45842</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
-      <c r="D54" s="4" t="str">
+      <c r="D54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L3</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54">
         <v>0</v>
       </c>
     </row>
@@ -1435,17 +1433,17 @@
       <c r="A55" s="1">
         <v>45842</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C55">
         <v>4</v>
       </c>
-      <c r="D55" s="4" t="str">
+      <c r="D55" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L4</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55">
         <v>0</v>
       </c>
     </row>
@@ -1453,17 +1451,17 @@
       <c r="A56" s="1">
         <v>45850</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
-      <c r="D56" s="4" t="str">
+      <c r="D56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT1</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56">
         <v>16</v>
       </c>
     </row>
@@ -1471,17 +1469,17 @@
       <c r="A57" s="1">
         <v>45850</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
-      <c r="D57" s="4" t="str">
+      <c r="D57" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT2</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57">
         <v>1</v>
       </c>
     </row>
@@ -1489,17 +1487,17 @@
       <c r="A58" s="1">
         <v>45850</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
-      <c r="D58" s="4" t="str">
+      <c r="D58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN1</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58">
         <v>18</v>
       </c>
     </row>
@@ -1507,17 +1505,17 @@
       <c r="A59" s="1">
         <v>45850</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
-      <c r="D59" s="4" t="str">
+      <c r="D59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN2</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59">
         <v>1</v>
       </c>
     </row>
@@ -1525,17 +1523,17 @@
       <c r="A60" s="1">
         <v>45850</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
-      <c r="D60" s="4" t="str">
+      <c r="D60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MN3</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60">
         <v>2</v>
       </c>
     </row>
@@ -1543,17 +1541,17 @@
       <c r="A61" s="1">
         <v>45850</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
-      <c r="D61" s="4" t="str">
+      <c r="D61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L1</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61">
         <v>1</v>
       </c>
     </row>
@@ -1561,17 +1559,17 @@
       <c r="A62" s="1">
         <v>45850</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C62">
         <v>2</v>
       </c>
-      <c r="D62" s="4" t="str">
+      <c r="D62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L2</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62">
         <v>2</v>
       </c>
     </row>
@@ -1579,17 +1577,17 @@
       <c r="A63" s="1">
         <v>45850</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C63">
         <v>3</v>
       </c>
-      <c r="D63" s="4" t="str">
+      <c r="D63" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L3</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63">
         <v>0</v>
       </c>
     </row>
@@ -1597,17 +1595,17 @@
       <c r="A64" s="1">
         <v>45850</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C64">
         <v>4</v>
       </c>
-      <c r="D64" s="4" t="str">
+      <c r="D64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L4</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64">
         <v>0</v>
       </c>
     </row>
@@ -1615,17 +1613,17 @@
       <c r="A65" s="1">
         <v>45857</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
-      <c r="D65" s="4" t="str">
+      <c r="D65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT1</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65">
         <v>16</v>
       </c>
     </row>
@@ -1633,17 +1631,17 @@
       <c r="A66" s="1">
         <v>45857</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C66">
         <v>2</v>
       </c>
-      <c r="D66" s="4" t="str">
+      <c r="D66" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MT2</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66">
         <v>2</v>
       </c>
     </row>
@@ -1651,17 +1649,17 @@
       <c r="A67" s="1">
         <v>45857</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
-      <c r="D67" s="4" t="str">
+      <c r="D67" s="3" t="str">
         <f t="shared" ref="D67:D130" si="1">B67&amp;C67</f>
         <v>MN1</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67">
         <v>18</v>
       </c>
     </row>
@@ -1669,17 +1667,17 @@
       <c r="A68" s="1">
         <v>45857</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C68">
         <v>2</v>
       </c>
-      <c r="D68" s="4" t="str">
+      <c r="D68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN2</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68">
         <v>2</v>
       </c>
     </row>
@@ -1687,17 +1685,17 @@
       <c r="A69" s="1">
         <v>45857</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C69">
         <v>3</v>
       </c>
-      <c r="D69" s="4" t="str">
+      <c r="D69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN3</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69">
         <v>3</v>
       </c>
     </row>
@@ -1705,17 +1703,17 @@
       <c r="A70" s="1">
         <v>45857</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
-      <c r="D70" s="4" t="str">
+      <c r="D70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L1</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70">
         <v>7</v>
       </c>
     </row>
@@ -1723,17 +1721,17 @@
       <c r="A71" s="1">
         <v>45857</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C71">
         <v>2</v>
       </c>
-      <c r="D71" s="4" t="str">
+      <c r="D71" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L2</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71">
         <v>4</v>
       </c>
     </row>
@@ -1741,17 +1739,17 @@
       <c r="A72" s="1">
         <v>45857</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C72">
         <v>3</v>
       </c>
-      <c r="D72" s="4" t="str">
+      <c r="D72" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L3</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72">
         <v>1</v>
       </c>
     </row>
@@ -1759,17 +1757,17 @@
       <c r="A73" s="1">
         <v>45857</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C73">
         <v>4</v>
       </c>
-      <c r="D73" s="4" t="str">
+      <c r="D73" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L4</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73">
         <v>0</v>
       </c>
     </row>
@@ -1777,17 +1775,17 @@
       <c r="A74" s="1">
         <v>45861</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
-      <c r="D74" s="4" t="str">
+      <c r="D74" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT1</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74">
         <v>17</v>
       </c>
     </row>
@@ -1795,17 +1793,17 @@
       <c r="A75" s="1">
         <v>45861</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C75">
         <v>2</v>
       </c>
-      <c r="D75" s="4" t="str">
+      <c r="D75" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT2</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75">
         <v>8</v>
       </c>
     </row>
@@ -1813,17 +1811,17 @@
       <c r="A76" s="1">
         <v>45861</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
-      <c r="D76" s="4" t="str">
+      <c r="D76" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN1</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76">
         <v>20</v>
       </c>
     </row>
@@ -1831,17 +1829,17 @@
       <c r="A77" s="1">
         <v>45861</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C77">
         <v>2</v>
       </c>
-      <c r="D77" s="4" t="str">
+      <c r="D77" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN2</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77">
         <v>9</v>
       </c>
     </row>
@@ -1849,17 +1847,17 @@
       <c r="A78" s="1">
         <v>45861</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C78">
         <v>3</v>
       </c>
-      <c r="D78" s="4" t="str">
+      <c r="D78" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN3</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78">
         <v>11</v>
       </c>
     </row>
@@ -1867,17 +1865,17 @@
       <c r="A79" s="1">
         <v>45861</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
-      <c r="D79" s="4" t="str">
+      <c r="D79" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L1</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79">
         <v>9.5</v>
       </c>
     </row>
@@ -1885,17 +1883,17 @@
       <c r="A80" s="1">
         <v>45861</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C80">
         <v>2</v>
       </c>
-      <c r="D80" s="4" t="str">
+      <c r="D80" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L2</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80">
         <v>5</v>
       </c>
     </row>
@@ -1903,17 +1901,17 @@
       <c r="A81" s="1">
         <v>45861</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C81">
         <v>3</v>
       </c>
-      <c r="D81" s="4" t="str">
+      <c r="D81" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L3</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81">
         <v>2.5</v>
       </c>
     </row>
@@ -1921,17 +1919,17 @@
       <c r="A82" s="1">
         <v>45861</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C82">
         <v>4</v>
       </c>
-      <c r="D82" s="4" t="str">
+      <c r="D82" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L4</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82">
         <v>0</v>
       </c>
     </row>
@@ -1939,17 +1937,17 @@
       <c r="A83" s="1">
         <v>45869</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
-      <c r="D83" s="4" t="str">
+      <c r="D83" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT1</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83">
         <v>25.5</v>
       </c>
     </row>
@@ -1957,17 +1955,17 @@
       <c r="A84" s="1">
         <v>45869</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C84">
         <v>2</v>
       </c>
-      <c r="D84" s="4" t="str">
+      <c r="D84" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT2</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84">
         <v>14</v>
       </c>
     </row>
@@ -1975,17 +1973,17 @@
       <c r="A85" s="1">
         <v>45869</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
-      <c r="D85" s="4" t="str">
+      <c r="D85" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN1</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85">
         <v>29</v>
       </c>
     </row>
@@ -1993,17 +1991,17 @@
       <c r="A86" s="1">
         <v>45869</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C86">
         <v>2</v>
       </c>
-      <c r="D86" s="4" t="str">
+      <c r="D86" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN2</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86">
         <v>14</v>
       </c>
     </row>
@@ -2011,17 +2009,17 @@
       <c r="A87" s="1">
         <v>45869</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C87">
         <v>3</v>
       </c>
-      <c r="D87" s="4" t="str">
+      <c r="D87" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN3</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87">
         <v>18</v>
       </c>
     </row>
@@ -2029,17 +2027,17 @@
       <c r="A88" s="1">
         <v>45869</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
-      <c r="D88" s="4" t="str">
+      <c r="D88" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L1</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88">
         <v>27</v>
       </c>
     </row>
@@ -2047,17 +2045,17 @@
       <c r="A89" s="1">
         <v>45869</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C89">
         <v>2</v>
       </c>
-      <c r="D89" s="4" t="str">
+      <c r="D89" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L2</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89">
         <v>21</v>
       </c>
     </row>
@@ -2065,17 +2063,17 @@
       <c r="A90" s="1">
         <v>45869</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C90">
         <v>3</v>
       </c>
-      <c r="D90" s="4" t="str">
+      <c r="D90" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L3</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90">
         <v>21</v>
       </c>
     </row>
@@ -2083,17 +2081,17 @@
       <c r="A91" s="1">
         <v>45869</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C91">
         <v>4</v>
       </c>
-      <c r="D91" s="4" t="str">
+      <c r="D91" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L4</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91">
         <v>9.5</v>
       </c>
     </row>
@@ -2101,17 +2099,17 @@
       <c r="A92" s="1">
         <v>45880</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
-      <c r="D92" s="4" t="str">
+      <c r="D92" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT1</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92">
         <v>19</v>
       </c>
     </row>
@@ -2119,17 +2117,17 @@
       <c r="A93" s="1">
         <v>45880</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C93">
         <v>2</v>
       </c>
-      <c r="D93" s="4" t="str">
+      <c r="D93" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT2</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93">
         <v>1</v>
       </c>
     </row>
@@ -2137,17 +2135,17 @@
       <c r="A94" s="1">
         <v>45880</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C94">
         <v>1</v>
       </c>
-      <c r="D94" s="4" t="str">
+      <c r="D94" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN1</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E94">
         <v>25.5</v>
       </c>
     </row>
@@ -2155,17 +2153,17 @@
       <c r="A95" s="1">
         <v>45880</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
-      <c r="D95" s="4" t="str">
+      <c r="D95" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN2</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E95">
         <v>8</v>
       </c>
     </row>
@@ -2173,17 +2171,17 @@
       <c r="A96" s="1">
         <v>45880</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C96">
         <v>3</v>
       </c>
-      <c r="D96" s="4" t="str">
+      <c r="D96" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN3</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96">
         <v>9</v>
       </c>
     </row>
@@ -2191,17 +2189,17 @@
       <c r="A97" s="1">
         <v>45880</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
-      <c r="D97" s="4" t="str">
+      <c r="D97" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L1</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97">
         <v>23.5</v>
       </c>
     </row>
@@ -2209,17 +2207,17 @@
       <c r="A98" s="1">
         <v>45880</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C98">
         <v>2</v>
       </c>
-      <c r="D98" s="4" t="str">
+      <c r="D98" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L2</v>
       </c>
-      <c r="E98" s="2">
+      <c r="E98">
         <v>14</v>
       </c>
     </row>
@@ -2227,17 +2225,17 @@
       <c r="A99" s="1">
         <v>45880</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C99">
         <v>3</v>
       </c>
-      <c r="D99" s="4" t="str">
+      <c r="D99" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L3</v>
       </c>
-      <c r="E99" s="2">
+      <c r="E99">
         <v>15</v>
       </c>
     </row>
@@ -2245,17 +2243,17 @@
       <c r="A100" s="1">
         <v>45880</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C100">
         <v>4</v>
       </c>
-      <c r="D100" s="4" t="str">
+      <c r="D100" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L4</v>
       </c>
-      <c r="E100" s="2">
+      <c r="E100">
         <v>2</v>
       </c>
     </row>
@@ -2263,17 +2261,17 @@
       <c r="A101" s="1">
         <v>45889</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
-      <c r="D101" s="4" t="str">
+      <c r="D101" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT1</v>
       </c>
-      <c r="E101" s="2">
+      <c r="E101">
         <v>14</v>
       </c>
     </row>
@@ -2281,17 +2279,17 @@
       <c r="A102" s="1">
         <v>45889</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
-      <c r="D102" s="4" t="str">
+      <c r="D102" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT2</v>
       </c>
-      <c r="E102" s="2">
+      <c r="E102">
         <v>0</v>
       </c>
     </row>
@@ -2299,17 +2297,17 @@
       <c r="A103" s="1">
         <v>45889</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
-      <c r="D103" s="4" t="str">
+      <c r="D103" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN1</v>
       </c>
-      <c r="E103" s="2">
+      <c r="E103">
         <v>10</v>
       </c>
     </row>
@@ -2317,17 +2315,17 @@
       <c r="A104" s="1">
         <v>45889</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C104">
         <v>2</v>
       </c>
-      <c r="D104" s="4" t="str">
+      <c r="D104" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN2</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104">
         <v>0</v>
       </c>
     </row>
@@ -2335,17 +2333,17 @@
       <c r="A105" s="1">
         <v>45889</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C105">
         <v>3</v>
       </c>
-      <c r="D105" s="4" t="str">
+      <c r="D105" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN3</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E105">
         <v>0.5</v>
       </c>
     </row>
@@ -2353,17 +2351,17 @@
       <c r="A106" s="1">
         <v>45889</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
-      <c r="D106" s="4" t="str">
+      <c r="D106" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L1</v>
       </c>
-      <c r="E106" s="2">
+      <c r="E106">
         <v>10</v>
       </c>
     </row>
@@ -2371,17 +2369,17 @@
       <c r="A107" s="1">
         <v>45889</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C107">
         <v>2</v>
       </c>
-      <c r="D107" s="4" t="str">
+      <c r="D107" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L2</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E107">
         <v>5</v>
       </c>
     </row>
@@ -2389,17 +2387,17 @@
       <c r="A108" s="1">
         <v>45889</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C108">
         <v>3</v>
       </c>
-      <c r="D108" s="4" t="str">
+      <c r="D108" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L3</v>
       </c>
-      <c r="E108" s="2">
+      <c r="E108">
         <v>4.5</v>
       </c>
     </row>
@@ -2407,17 +2405,17 @@
       <c r="A109" s="1">
         <v>45889</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C109">
         <v>4</v>
       </c>
-      <c r="D109" s="4" t="str">
+      <c r="D109" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L4</v>
       </c>
-      <c r="E109" s="2">
+      <c r="E109">
         <v>0</v>
       </c>
     </row>
@@ -2425,17 +2423,17 @@
       <c r="A110" s="1">
         <v>45900</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
-      <c r="D110" s="4" t="str">
+      <c r="D110" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT1</v>
       </c>
-      <c r="E110" s="2">
+      <c r="E110">
         <v>14</v>
       </c>
     </row>
@@ -2443,17 +2441,17 @@
       <c r="A111" s="1">
         <v>45900</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C111">
         <v>2</v>
       </c>
-      <c r="D111" s="4" t="str">
+      <c r="D111" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT2</v>
       </c>
-      <c r="E111" s="2">
+      <c r="E111">
         <v>7</v>
       </c>
     </row>
@@ -2461,17 +2459,17 @@
       <c r="A112" s="1">
         <v>45900</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
-      <c r="D112" s="4" t="str">
+      <c r="D112" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN1</v>
       </c>
-      <c r="E112" s="2">
+      <c r="E112">
         <v>13</v>
       </c>
     </row>
@@ -2479,17 +2477,17 @@
       <c r="A113" s="1">
         <v>45900</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C113">
         <v>2</v>
       </c>
-      <c r="D113" s="4" t="str">
+      <c r="D113" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN2</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113">
         <v>0</v>
       </c>
     </row>
@@ -2497,17 +2495,17 @@
       <c r="A114" s="1">
         <v>45900</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C114">
         <v>3</v>
       </c>
-      <c r="D114" s="4" t="str">
+      <c r="D114" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN3</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E114">
         <v>1</v>
       </c>
     </row>
@@ -2515,17 +2513,17 @@
       <c r="A115" s="1">
         <v>45900</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C115">
         <v>1</v>
       </c>
-      <c r="D115" s="4" t="str">
+      <c r="D115" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L1</v>
       </c>
-      <c r="E115" s="2">
+      <c r="E115">
         <v>12</v>
       </c>
     </row>
@@ -2533,17 +2531,17 @@
       <c r="A116" s="1">
         <v>45900</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C116">
         <v>2</v>
       </c>
-      <c r="D116" s="4" t="str">
+      <c r="D116" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L2</v>
       </c>
-      <c r="E116" s="2">
+      <c r="E116">
         <v>7</v>
       </c>
     </row>
@@ -2551,17 +2549,17 @@
       <c r="A117" s="1">
         <v>45900</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C117">
         <v>3</v>
       </c>
-      <c r="D117" s="4" t="str">
+      <c r="D117" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L3</v>
       </c>
-      <c r="E117" s="2">
+      <c r="E117">
         <v>6</v>
       </c>
     </row>
@@ -2569,17 +2567,17 @@
       <c r="A118" s="1">
         <v>45900</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C118">
         <v>4</v>
       </c>
-      <c r="D118" s="4" t="str">
+      <c r="D118" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L4</v>
       </c>
-      <c r="E118" s="2">
+      <c r="E118">
         <v>0</v>
       </c>
     </row>
@@ -2587,17 +2585,17 @@
       <c r="A119" s="1">
         <v>45908</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
-      <c r="D119" s="4" t="str">
+      <c r="D119" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT1</v>
       </c>
-      <c r="E119" s="2">
+      <c r="E119">
         <v>12</v>
       </c>
     </row>
@@ -2605,17 +2603,17 @@
       <c r="A120" s="1">
         <v>45908</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C120">
         <v>2</v>
       </c>
-      <c r="D120" s="4" t="str">
+      <c r="D120" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT2</v>
       </c>
-      <c r="E120" s="2">
+      <c r="E120">
         <v>18</v>
       </c>
     </row>
@@ -2623,17 +2621,17 @@
       <c r="A121" s="1">
         <v>45908</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
-      <c r="D121" s="4" t="str">
+      <c r="D121" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN1</v>
       </c>
-      <c r="E121" s="2">
+      <c r="E121">
         <v>19</v>
       </c>
     </row>
@@ -2641,17 +2639,17 @@
       <c r="A122" s="1">
         <v>45908</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C122">
         <v>2</v>
       </c>
-      <c r="D122" s="4" t="str">
+      <c r="D122" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN2</v>
       </c>
-      <c r="E122" s="2">
+      <c r="E122">
         <v>4.5</v>
       </c>
     </row>
@@ -2659,17 +2657,17 @@
       <c r="A123" s="1">
         <v>45908</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C123">
         <v>3</v>
       </c>
-      <c r="D123" s="4" t="str">
+      <c r="D123" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN3</v>
       </c>
-      <c r="E123" s="2">
+      <c r="E123">
         <v>4</v>
       </c>
     </row>
@@ -2677,17 +2675,17 @@
       <c r="A124" s="1">
         <v>45908</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
-      <c r="D124" s="4" t="str">
+      <c r="D124" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L1</v>
       </c>
-      <c r="E124" s="2">
+      <c r="E124">
         <v>16.5</v>
       </c>
     </row>
@@ -2695,17 +2693,17 @@
       <c r="A125" s="1">
         <v>45908</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C125">
         <v>2</v>
       </c>
-      <c r="D125" s="4" t="str">
+      <c r="D125" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L2</v>
       </c>
-      <c r="E125" s="2">
+      <c r="E125">
         <v>12</v>
       </c>
     </row>
@@ -2713,17 +2711,17 @@
       <c r="A126" s="1">
         <v>45908</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B126" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C126">
         <v>3</v>
       </c>
-      <c r="D126" s="4" t="str">
+      <c r="D126" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L3</v>
       </c>
-      <c r="E126" s="2">
+      <c r="E126">
         <v>11</v>
       </c>
     </row>
@@ -2731,17 +2729,17 @@
       <c r="A127" s="1">
         <v>45908</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C127">
         <v>4</v>
       </c>
-      <c r="D127" s="4" t="str">
+      <c r="D127" s="3" t="str">
         <f t="shared" si="1"/>
         <v>L4</v>
       </c>
-      <c r="E127" s="2">
+      <c r="E127">
         <v>2</v>
       </c>
     </row>
@@ -2749,17 +2747,17 @@
       <c r="A128" s="1">
         <v>45918</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
-      <c r="D128" s="4" t="str">
+      <c r="D128" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT1</v>
       </c>
-      <c r="E128" s="2">
+      <c r="E128">
         <v>14</v>
       </c>
     </row>
@@ -2767,17 +2765,17 @@
       <c r="A129" s="1">
         <v>45918</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C129">
         <v>2</v>
       </c>
-      <c r="D129" s="4" t="str">
+      <c r="D129" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MT2</v>
       </c>
-      <c r="E129" s="2">
+      <c r="E129">
         <v>4</v>
       </c>
     </row>
@@ -2785,17 +2783,17 @@
       <c r="A130" s="1">
         <v>45918</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
-      <c r="D130" s="4" t="str">
+      <c r="D130" s="3" t="str">
         <f t="shared" si="1"/>
         <v>MN1</v>
       </c>
-      <c r="E130" s="2">
+      <c r="E130">
         <v>11</v>
       </c>
     </row>
@@ -2803,17 +2801,17 @@
       <c r="A131" s="1">
         <v>45918</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C131">
         <v>2</v>
       </c>
-      <c r="D131" s="4" t="str">
+      <c r="D131" s="3" t="str">
         <f t="shared" ref="D131:D154" si="2">B131&amp;C131</f>
         <v>MN2</v>
       </c>
-      <c r="E131" s="2">
+      <c r="E131">
         <v>0</v>
       </c>
     </row>
@@ -2821,17 +2819,17 @@
       <c r="A132" s="1">
         <v>45918</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B132" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C132">
         <v>3</v>
       </c>
-      <c r="D132" s="4" t="str">
+      <c r="D132" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MN3</v>
       </c>
-      <c r="E132" s="2">
+      <c r="E132">
         <v>0</v>
       </c>
     </row>
@@ -2839,17 +2837,17 @@
       <c r="A133" s="1">
         <v>45918</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
-      <c r="D133" s="4" t="str">
+      <c r="D133" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L1</v>
       </c>
-      <c r="E133" s="2">
+      <c r="E133">
         <v>9</v>
       </c>
     </row>
@@ -2857,17 +2855,17 @@
       <c r="A134" s="1">
         <v>45918</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B134" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C134">
         <v>2</v>
       </c>
-      <c r="D134" s="4" t="str">
+      <c r="D134" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L2</v>
       </c>
-      <c r="E134" s="3">
+      <c r="E134" s="2">
         <v>11</v>
       </c>
     </row>
@@ -2875,17 +2873,17 @@
       <c r="A135" s="1">
         <v>45918</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C135">
         <v>3</v>
       </c>
-      <c r="D135" s="4" t="str">
+      <c r="D135" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L3</v>
       </c>
-      <c r="E135" s="3">
+      <c r="E135" s="2">
         <v>7</v>
       </c>
     </row>
@@ -2893,179 +2891,179 @@
       <c r="A136" s="1">
         <v>45918</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C136">
         <v>4</v>
       </c>
-      <c r="D136" s="4" t="str">
+      <c r="D136" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L4</v>
       </c>
-      <c r="E136" s="2">
+      <c r="E136">
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B137" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B137" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
-      <c r="D137" s="4" t="str">
+      <c r="D137" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MT1</v>
       </c>
-      <c r="E137" s="2">
+      <c r="E137">
         <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B138" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B138" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C138">
         <v>2</v>
       </c>
-      <c r="D138" s="4" t="str">
+      <c r="D138" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MT2</v>
       </c>
-      <c r="E138" s="2">
+      <c r="E138">
         <v>13</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B139" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B139" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
-      <c r="D139" s="4" t="str">
+      <c r="D139" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MN1</v>
       </c>
-      <c r="E139" s="2">
+      <c r="E139">
         <v>17.5</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B140" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B140" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C140">
         <v>2</v>
       </c>
-      <c r="D140" s="4" t="str">
+      <c r="D140" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MN2</v>
       </c>
-      <c r="E140" s="2">
+      <c r="E140">
         <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B141" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B141" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C141">
         <v>3</v>
       </c>
-      <c r="D141" s="4" t="str">
+      <c r="D141" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MN3</v>
       </c>
-      <c r="E141" s="2">
+      <c r="E141">
         <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B142" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B142" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
-      <c r="D142" s="4" t="str">
+      <c r="D142" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L1</v>
       </c>
-      <c r="E142" s="2">
+      <c r="E142">
         <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B143" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C143">
         <v>2</v>
       </c>
-      <c r="D143" s="4" t="str">
+      <c r="D143" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L2</v>
       </c>
-      <c r="E143" s="2">
+      <c r="E143">
         <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B144" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B144" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C144">
         <v>3</v>
       </c>
-      <c r="D144" s="4" t="str">
+      <c r="D144" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L3</v>
       </c>
-      <c r="E144" s="2">
+      <c r="E144">
         <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>45559</v>
-      </c>
-      <c r="B145" s="4" t="s">
+        <v>45924</v>
+      </c>
+      <c r="B145" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C145">
         <v>4</v>
       </c>
-      <c r="D145" s="4" t="str">
+      <c r="D145" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L4</v>
       </c>
-      <c r="E145" s="2">
+      <c r="E145">
         <v>4</v>
       </c>
     </row>
@@ -3073,17 +3071,17 @@
       <c r="A146" s="1">
         <v>45929</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
-      <c r="D146" s="4" t="str">
+      <c r="D146" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MT1</v>
       </c>
-      <c r="E146" s="2">
+      <c r="E146">
         <v>21</v>
       </c>
     </row>
@@ -3091,17 +3089,17 @@
       <c r="A147" s="1">
         <v>45929</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C147">
         <v>2</v>
       </c>
-      <c r="D147" s="4" t="str">
+      <c r="D147" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MT2</v>
       </c>
-      <c r="E147" s="2">
+      <c r="E147">
         <v>11</v>
       </c>
     </row>
@@ -3109,17 +3107,17 @@
       <c r="A148" s="1">
         <v>45929</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C148">
         <v>1</v>
       </c>
-      <c r="D148" s="4" t="str">
+      <c r="D148" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MN1</v>
       </c>
-      <c r="E148" s="2">
+      <c r="E148">
         <v>25</v>
       </c>
     </row>
@@ -3127,17 +3125,17 @@
       <c r="A149" s="1">
         <v>45929</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C149">
         <v>2</v>
       </c>
-      <c r="D149" s="4" t="str">
+      <c r="D149" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MN2</v>
       </c>
-      <c r="E149" s="2">
+      <c r="E149">
         <v>11</v>
       </c>
     </row>
@@ -3145,17 +3143,17 @@
       <c r="A150" s="1">
         <v>45929</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B150" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C150">
         <v>3</v>
       </c>
-      <c r="D150" s="4" t="str">
+      <c r="D150" s="3" t="str">
         <f t="shared" si="2"/>
         <v>MN3</v>
       </c>
-      <c r="E150" s="2">
+      <c r="E150">
         <v>10</v>
       </c>
     </row>
@@ -3163,17 +3161,17 @@
       <c r="A151" s="1">
         <v>45929</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C151">
         <v>1</v>
       </c>
-      <c r="D151" s="4" t="str">
+      <c r="D151" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L1</v>
       </c>
-      <c r="E151" s="2">
+      <c r="E151">
         <v>22.5</v>
       </c>
     </row>
@@ -3181,17 +3179,17 @@
       <c r="A152" s="1">
         <v>45929</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B152" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C152">
         <v>2</v>
       </c>
-      <c r="D152" s="4" t="str">
+      <c r="D152" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L2</v>
       </c>
-      <c r="E152" s="2">
+      <c r="E152">
         <v>15</v>
       </c>
     </row>
@@ -3199,17 +3197,17 @@
       <c r="A153" s="1">
         <v>45929</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B153" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C153">
         <v>3</v>
       </c>
-      <c r="D153" s="4" t="str">
+      <c r="D153" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L3</v>
       </c>
-      <c r="E153" s="2">
+      <c r="E153">
         <v>13</v>
       </c>
     </row>
@@ -3217,17 +3215,17 @@
       <c r="A154" s="1">
         <v>45929</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C154">
         <v>4</v>
       </c>
-      <c r="D154" s="4" t="str">
+      <c r="D154" s="3" t="str">
         <f t="shared" si="2"/>
         <v>L4</v>
       </c>
-      <c r="E154" s="2">
+      <c r="E154">
         <v>9</v>
       </c>
     </row>

</xml_diff>